<commit_message>
WIP: completed scaffolding for xlsx reader, missing tests
</commit_message>
<xml_diff>
--- a/tests/xl_workbooks/t.xlsx
+++ b/tests/xl_workbooks/t.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eddiec11us\dev_apps\reporter\tests\tests_safe_read_xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eddiec11us\dev_apps\reporter\tests\xl_workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6DA1B29-FE00-48BD-8421-CE7CBCE35040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2E5C1-0606-4CF5-B432-EB7020B7FB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9015" yWindow="5055" windowWidth="28485" windowHeight="15285" activeTab="1" xr2:uid="{EBD63F48-45C2-4EF3-ADEC-6E257A95D29A}"/>
+    <workbookView xWindow="9015" yWindow="5055" windowWidth="28485" windowHeight="15285" xr2:uid="{EBD63F48-45C2-4EF3-ADEC-6E257A95D29A}"/>
   </bookViews>
   <sheets>
-    <sheet name="foo" sheetId="1" r:id="rId1"/>
-    <sheet name="bar" sheetId="2" r:id="rId2"/>
+    <sheet name="bar" sheetId="2" r:id="rId1"/>
+    <sheet name="foo" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -409,18 +409,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59ADECD-A82A-41B3-B53A-823A0924993C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCE3C66-63FD-4160-80C3-394916D686D9}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -464,4 +452,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59ADECD-A82A-41B3-B53A-823A0924993C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tests for safe reader complete
</commit_message>
<xml_diff>
--- a/tests/xl_workbooks/t.xlsx
+++ b/tests/xl_workbooks/t.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eddiec11us\dev_apps\reporter\tests\xl_workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2E5C1-0606-4CF5-B432-EB7020B7FB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805042B8-2AC6-4797-BFB9-DFCDC43F4EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9015" yWindow="5055" windowWidth="28485" windowHeight="15285" xr2:uid="{EBD63F48-45C2-4EF3-ADEC-6E257A95D29A}"/>
+    <workbookView xWindow="9015" yWindow="5055" windowWidth="28485" windowHeight="15285" activeTab="1" xr2:uid="{EBD63F48-45C2-4EF3-ADEC-6E257A95D29A}"/>
   </bookViews>
   <sheets>
     <sheet name="bar" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>spam</t>
   </si>
@@ -59,6 +59,27 @@
   </si>
   <si>
     <t>ham</t>
+  </si>
+  <si>
+    <t>karina</t>
+  </si>
+  <si>
+    <t>kayla</t>
+  </si>
+  <si>
+    <t>baby</t>
+  </si>
+  <si>
+    <t>mom</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>og</t>
   </si>
 </sst>
 </file>
@@ -412,7 +433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCE3C66-63FD-4160-80C3-394916D686D9}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -456,12 +479,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59ADECD-A82A-41B3-B53A-823A0924993C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>